<commit_message>
added some steps for filtering out non protein-coding genes
</commit_message>
<xml_diff>
--- a/Gene_lists/NMD_genes/nmd_genes_2018.xlsx
+++ b/Gene_lists/NMD_genes/nmd_genes_2018.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubydawes/Documents/GitHub/Honours_Project/Project/Gene_lists/NMD_genes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubydawes/Documents/GitHub/Constraint_Project/Gene_lists/NMD_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C21581-2C0A-4645-B233-E1285DCD7C8A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D399C22C-9E64-204C-8F20-520B22AB96C0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="13120" windowHeight="6100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13140" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$A$636</definedName>
+  </definedNames>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="638">
   <si>
     <t>AARS</t>
   </si>
@@ -1928,6 +1931,12 @@
   </si>
   <si>
     <t>gene</t>
+  </si>
+  <si>
+    <t>pubmed yes</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -2261,9 +2270,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A636"/>
+  <dimension ref="A1:B636"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2987,82 +2998,85 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -3547,82 +3561,85 @@
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B270" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>270</v>
       </c>
@@ -3787,82 +3804,85 @@
         <v>302</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B311" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>318</v>
       </c>
@@ -4187,82 +4207,85 @@
         <v>382</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B390" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>398</v>
       </c>
@@ -5448,6 +5471,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A636" xr:uid="{7A97A25F-870A-C64F-BFCE-4E585D0F6EC1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>